<commit_message>
Updated preprocessing datasets and imputation process.
</commit_message>
<xml_diff>
--- a/data/8 cohorts codebook.xlsx
+++ b/data/8 cohorts codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JGUO258\Documents\JGUO\papers repo\diabetes_subphenotypes_predictors\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A63859-FFC5-4A00-A586-A8386F77400E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B4F958-2197-4C7F-A5F0-F7F96D78DB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="79">
   <si>
     <t xml:space="preserve">Harmonized </t>
   </si>
@@ -57,9 +57,6 @@
     <t>mesa</t>
   </si>
   <si>
-    <t>dpp/dppos</t>
-  </si>
-  <si>
     <t>hrs</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>apo_b</t>
   </si>
   <si>
-    <t>bsage</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -240,35 +234,41 @@
     <t>Medication</t>
   </si>
   <si>
-    <t>cholesterol</t>
-  </si>
-  <si>
     <t>statins</t>
   </si>
   <si>
-    <t>anti-htn</t>
-  </si>
-  <si>
     <t>anti-psychotics</t>
   </si>
   <si>
-    <t>anti-depression</t>
-  </si>
-  <si>
     <t>insulin</t>
   </si>
   <si>
-    <t>medication_dm</t>
-  </si>
-  <si>
     <t>wave (character)</t>
+  </si>
+  <si>
+    <t>bsage + visit time period</t>
+  </si>
+  <si>
+    <t>med_chol_use</t>
+  </si>
+  <si>
+    <t>med_bp_use</t>
+  </si>
+  <si>
+    <t>med_dm_use</t>
+  </si>
+  <si>
+    <t>dppos</t>
+  </si>
+  <si>
+    <t>anti-depressant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +285,20 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -348,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -369,14 +383,12 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,7 +672,7 @@
   <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -699,15 +711,15 @@
         <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" s="11">
         <v>601</v>
@@ -739,7 +751,7 @@
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="12">
         <v>22925</v>
@@ -771,7 +783,7 @@
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -834,25 +846,25 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
         <v>51</v>
-      </c>
-      <c r="F7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" t="s">
-        <v>53</v>
       </c>
       <c r="H7" t="s">
         <v>3</v>
@@ -863,1065 +875,1090 @@
     </row>
     <row r="8" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>46</v>
+        <v>12</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" t="s">
-        <v>69</v>
+        <v>14</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
-      </c>
-      <c r="I11" t="s">
-        <v>69</v>
+        <v>54</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" t="s">
         <v>50</v>
       </c>
-      <c r="E14" t="s">
-        <v>52</v>
-      </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>22</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>22</v>
       </c>
-      <c r="D15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="D16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="G16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="16"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" t="s">
+        <v>76</v>
+      </c>
+      <c r="I18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" t="s">
+        <v>75</v>
+      </c>
+      <c r="I20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="15" t="s">
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="17"/>
-    </row>
-    <row r="18" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="19"/>
-    </row>
-    <row r="19" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="19"/>
-    </row>
-    <row r="20" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-    </row>
-    <row r="21" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-    </row>
-    <row r="22" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-    </row>
-    <row r="23" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-    </row>
-    <row r="24" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F39" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H39" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I43" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D45" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I45" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I46" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F47" t="s">
+        <v>40</v>
+      </c>
+      <c r="G47" t="s">
+        <v>40</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>41</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H48" t="s">
         <v>41</v>
       </c>
-      <c r="D47" t="s">
-        <v>41</v>
-      </c>
-      <c r="E47" t="s">
-        <v>41</v>
-      </c>
-      <c r="F47" t="s">
-        <v>41</v>
-      </c>
-      <c r="G47" t="s">
-        <v>41</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I47" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" t="s">
-        <v>42</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H48" t="s">
-        <v>42</v>
-      </c>
       <c r="I48" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+      <c r="A49" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D49" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" t="s">
+        <v>43</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I49" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="B50" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" t="s">
         <v>44</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E50" t="s">
         <v>44</v>
       </c>
-      <c r="F49" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H49" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I49" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>45</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D50" t="s">
-        <v>45</v>
-      </c>
-      <c r="E50" t="s">
-        <v>45</v>
-      </c>
       <c r="F50" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H50" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I50" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C51" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D51" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E51" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F51" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G51" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H51" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C52" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D52" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E52" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F52" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G52" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H52" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned and harmonized 8 cohorts data; re-run analysis.
</commit_message>
<xml_diff>
--- a/data/8 cohorts codebook.xlsx
+++ b/data/8 cohorts codebook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JGUO258\Documents\JGUO\papers repo\diabetes_subphenotypes_predictors\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B4F958-2197-4C7F-A5F0-F7F96D78DB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC58024D-EFF0-4D2A-B013-0EA96D776522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="81">
   <si>
     <t xml:space="preserve">Harmonized </t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>anti-depressant</t>
+  </si>
+  <si>
+    <t>race_clean</t>
+  </si>
+  <si>
+    <t>urinealbumin/urinecreatinine</t>
   </si>
 </sst>
 </file>
@@ -362,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -389,6 +395,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1025,7 +1032,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
@@ -1780,8 +1787,8 @@
       <c r="E46" t="s">
         <v>39</v>
       </c>
-      <c r="F46" s="9" t="s">
-        <v>45</v>
+      <c r="F46" s="20" t="s">
+        <v>80</v>
       </c>
       <c r="G46" t="s">
         <v>39</v>

</xml_diff>